<commit_message>
added python script to brute force password reset
</commit_message>
<xml_diff>
--- a/case_study.xlsx
+++ b/case_study.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\personal\projects\FOR_INTERVIEWS\innoscripta\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED85FFE6-D1C9-49D9-B334-6D7E99CBE7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test cases" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="preconditions+shared_steps" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +26,158 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+  <si>
+    <t>Test Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Pre Condition</t>
+  </si>
+  <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>Test Steps</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Test designed By</t>
+  </si>
+  <si>
+    <t>Valid creds Facebook login</t>
+  </si>
+  <si>
+    <t>Verify Login with the Valid username and password on Facebook.com</t>
+  </si>
+  <si>
+    <t>Valid Username and Password</t>
+  </si>
+  <si>
+    <t>username : chunky
+password : panday123</t>
+  </si>
+  <si>
+    <t>1. Open Facebook.com
+2. Enter Username and Password
+3. Verify the Facebook Dashboard is loaded.</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>Pramod</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Defect Link</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Dashboard should load fine</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Step Name</t>
+  </si>
+  <si>
+    <t>Log in</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>1) In incognito mode go to https://techshopbd.com/sign-in
+2) Enter the email in the "Email" field and click "Next"
+3) Enter the password in the "Password" field and click the blue "Login" button.</t>
+  </si>
+  <si>
+    <t>Feature/Module</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Verify user can do the registration process successfully.</t>
+  </si>
+  <si>
+    <t>Verify a new user can register with a facebook account.</t>
+  </si>
+  <si>
+    <t>Successful registration (new google account)</t>
+  </si>
+  <si>
+    <t>Successful registration (new facebook account)</t>
+  </si>
+  <si>
+    <t>Verify a new user can register with a google account.</t>
+  </si>
+  <si>
+    <t>Successful registration (normal account)</t>
+  </si>
+  <si>
+    <t>Sign in with "Google" account, after normal account creation</t>
+  </si>
+  <si>
+    <t>Verify a user that initially registered normally with a google email, can still use and sign in through the "Google" button.</t>
+  </si>
+  <si>
+    <t>Registration/Sign-in</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>WHAT IS THE EXPECTED BEHAVIOR?</t>
+  </si>
+  <si>
+    <t>Registration fields constraints</t>
+  </si>
+  <si>
+    <t>Validate the behavior and constraints of the "Full Name", "Phone", "Password" and "OTP Verification" fields, during registration.
+Verify correct error messages are showed to the user.</t>
+  </si>
+  <si>
+    <t>Registration with empty fields</t>
+  </si>
+  <si>
+    <t>Verify a user can't register if any of the fields are empty</t>
+  </si>
+  <si>
+    <t>Registration with existing phone number</t>
+  </si>
+  <si>
+    <t>A user can't register with a phone number that was already registered.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +185,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Lato"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Lato"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -45,17 +247,226 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +477,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F555CF1F-18F6-4908-8428-36DB19ADCD4B}" name="Table3" displayName="Table3" ref="A1:C16" totalsRowShown="0" tableBorderDxfId="3">
+  <autoFilter ref="A1:C16" xr:uid="{F555CF1F-18F6-4908-8428-36DB19ADCD4B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D5C7C80C-F4D5-47BF-B5C9-C5E52D89E57F}" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E5C6B5B4-FFE5-4F22-AF3F-44D74826FC09}" name="Step Name" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{F17CC22E-1116-4BEA-BB3C-138D8E8AB89B}" name="Details" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +753,365 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2607C0-B33A-4A87-8C6B-2CEF4B89D541}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="64" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19">
+        <v>4</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19">
+        <v>5</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="19">
+        <v>6</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="19">
+        <v>7</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="19">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FBFEDB-FA26-47D2-8CE6-2036C94BD4AC}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" style="4" customWidth="1"/>
+    <col min="2" max="13" width="15.7109375" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="153" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="http://facebook.com/" xr:uid="{93F6CE83-A696-46D8-B5C4-B6881E7F04E1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA9EA0BE-E884-4667-9F0F-C24E5314222F}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test cases and test scripts
</commit_message>
<xml_diff>
--- a/case_study.xlsx
+++ b/case_study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\personal\projects\FOR_INTERVIEWS\innoscripta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED85FFE6-D1C9-49D9-B334-6D7E99CBE7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724B77C8-FBC4-4B10-9924-275DC5ACDD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>Test Name</t>
   </si>
@@ -41,42 +41,9 @@
     <t>TestData</t>
   </si>
   <si>
-    <t>Test Steps</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
     <t>Test designed By</t>
   </si>
   <si>
-    <t>Valid creds Facebook login</t>
-  </si>
-  <si>
-    <t>Verify Login with the Valid username and password on Facebook.com</t>
-  </si>
-  <si>
-    <t>Valid Username and Password</t>
-  </si>
-  <si>
-    <t>username : chunky
-password : panday123</t>
-  </si>
-  <si>
-    <t>1. Open Facebook.com
-2. Enter Username and Password
-3. Verify the Facebook Dashboard is loaded.</t>
-  </si>
-  <si>
-    <t>P0</t>
-  </si>
-  <si>
-    <t>Pramod</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
     <t>Actual Result</t>
   </si>
   <si>
@@ -87,12 +54,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>Dashboard should load fine</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
   <si>
     <t>NA</t>
@@ -171,13 +132,170 @@
   </si>
   <si>
     <t>A user can't register with a phone number that was already registered.</t>
+  </si>
+  <si>
+    <t>Registration (constraints)</t>
+  </si>
+  <si>
+    <t>Test Type</t>
+  </si>
+  <si>
+    <t>Have a non registered email address and a non registered phone number. (phone number can be fake)</t>
+  </si>
+  <si>
+    <t>Ariel Agranovich</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Using an incognito mode, go to the web site https://techshopbd.com/</t>
+  </si>
+  <si>
+    <t>User is redirected to the sign in page.
+1) The page path is "/sign-in".
+2) The options to sign in with Facebook/Google are present.
+3) An email text field is available, with place holder text of "Enter your email".
+4) A blue "Next" button is available and enabled.</t>
+  </si>
+  <si>
+    <t>Click the "Sign in" button.</t>
+  </si>
+  <si>
+    <t>Site loads and the "Sign in" button is present.</t>
+  </si>
+  <si>
+    <t>Input the unregistered email address and press the "Next" button.</t>
+  </si>
+  <si>
+    <t>Successful log-in with registered user (normal account)</t>
+  </si>
+  <si>
+    <t>User can use a registered email + password to log in into his existing account.</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>Fill all the required fields, except the "OTP Verification" field.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) The user sees a "Sign Up to TechShop" box.
+2) The next fields/elements are now visable:
+         - An empty "Full Name" field.
+         - The "Email" text field is now grayed out and uneditable.
+         - An empty "Phone" field (with the placeholder "(e.g., 8801234567890 or 01234567890)"
+         - An empty "Password" field with a round blue info icon on the header, and an eye icon on the right of the field.
+         - A gray line under the password field.
+         - An empty "OTP Verification" field with a place holder "Enter OTP" and a blue "Send OTP" button on the right.
+</t>
+  </si>
+  <si>
+    <t>Click on the "Send OTP" button.</t>
+  </si>
+  <si>
+    <t>When filling the password notice that:
+1) A red text with "Missing: …." appears, indicates what requirements are not yet met in the password
+2) The gray bar changes colors, depending on how many conditions are met. The bar changes colors following this logic:
+- Gray: no conditions are met
+- Red: 1 condition is met
+- Yellow (bar is half filled) : 2 conditions are met
+- Yellow (bar is 3/4 filled) : 3 conditions are met
+- Green: All conditions are met. The "Missing..." text is replaced with "Strong password! All requirements met."
+3) Only after all password conditions are met, The "Send OTP" Button becomes clickable.</t>
+  </si>
+  <si>
+    <t>The page loads a bit and some new elements appear on screen:
+- A green text "OTP sent Your Email successfully!!" appears for a short time in the top (under Facebook/Google buttons)
+- The "Send OTP" button changed to "Resend OTP in 120s" and is now disabled.
+- A running timer that starts at 120s "Resend OTP Available in …"
+- A "Remember me" checkbox appears.</t>
+  </si>
+  <si>
+    <t>Check the inbox of the email you used and look for an email with the OTP code.</t>
+  </si>
+  <si>
+    <t>The email sender is "info@techshopbd.com".
+The message in the email is:
+"""
+Your OTP code is XXXXXX. It is valid for 10 minutes.
+Thanks, Techshopbd.com
+"""
+(Where the XXXXXX is a 6 digit code.)</t>
+  </si>
+  <si>
+    <t>Input the code from the email to the "OTP Verification" field and click "Registration".</t>
+  </si>
+  <si>
+    <t>1) A green text "OTP Verified! Completing registration…" is showed in the top of the sign-up box.
+2) The user is redirected to the hope page (https://techshopbd.com/) (NO PATH)
+3) The user is logged in and sees his name that he filled during registration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "OTP resent successfully!!" </t>
+  </si>
+  <si>
+    <t>step_id</t>
+  </si>
+  <si>
+    <t>Have a known, already registered phone number (like "01234567890")</t>
+  </si>
+  <si>
+    <r>
+      <t>Do</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> steps 1-4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test_id: 1</t>
+    </r>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Replace the phone number in the "Phone" field with the already registered phone number.</t>
+  </si>
+  <si>
+    <t>1) A red text "Phone Number Already Exists. Please use another phone number." appears on the top of the registration form.
+2) No email with OTP code was received.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +329,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -224,8 +350,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,8 +391,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -327,19 +492,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -349,19 +546,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -378,6 +569,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -388,13 +582,110 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -754,141 +1045,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2607C0-B33A-4A87-8C6B-2CEF4B89D541}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="64" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="3" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="64" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
+        <v>4</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C9" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17">
+        <v>7</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C10" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19">
-        <v>4</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19">
-        <v>5</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
-        <v>6</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19">
-        <v>7</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19">
+      <c r="D10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17">
         <v>8</v>
       </c>
     </row>
@@ -899,102 +1213,315 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FBFEDB-FA26-47D2-8CE6-2036C94BD4AC}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="4" customWidth="1"/>
-    <col min="2" max="13" width="15.7109375" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="5.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="88.140625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="111.7109375" style="23" customWidth="1"/>
+    <col min="9" max="13" width="15.7109375" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G2" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G3" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="33"/>
+    </row>
+    <row r="4" spans="1:13" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G4" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="33"/>
+    </row>
+    <row r="5" spans="1:13" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="28">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G5" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="33"/>
+    </row>
+    <row r="6" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="28">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="G6" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="33"/>
+    </row>
+    <row r="7" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="28">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="153" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="G7" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="33"/>
+    </row>
+    <row r="8" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40">
+        <v>7</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="44"/>
+    </row>
+    <row r="9" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="48">
+        <v>6</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="48"/>
+      <c r="F9" s="51">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>21</v>
+      <c r="G9" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="48"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="51">
+        <v>2</v>
+      </c>
+      <c r="G10" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+    </row>
+    <row r="11" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="48"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="51">
+        <v>3</v>
+      </c>
+      <c r="G11" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H14" s="23" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="M2:M8"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://facebook.com/" xr:uid="{93F6CE83-A696-46D8-B5C4-B6881E7F04E1}"/>
+    <hyperlink ref="G2" r:id="rId1" display="Go to the web site https://techshopbd.com/" xr:uid="{D0D98396-E89F-4498-BC22-79FF13FA3777}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1006,107 +1533,107 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="54.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>22</v>
+      <c r="A1" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>26</v>
+      <c r="B2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="16"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more test cases work and organization
</commit_message>
<xml_diff>
--- a/case_study.xlsx
+++ b/case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\personal\projects\FOR_INTERVIEWS\innoscripta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724B77C8-FBC4-4B10-9924-275DC5ACDD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE7E069-9084-45D7-A187-1698EB3CDE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test cases" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="156">
   <si>
     <t>Test Name</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>ID</t>
@@ -116,10 +113,6 @@
   </si>
   <si>
     <t>Registration fields constraints</t>
-  </si>
-  <si>
-    <t>Validate the behavior and constraints of the "Full Name", "Phone", "Password" and "OTP Verification" fields, during registration.
-Verify correct error messages are showed to the user.</t>
   </si>
   <si>
     <t>Registration with empty fields</t>
@@ -290,12 +283,325 @@
     <t>1) A red text "Phone Number Already Exists. Please use another phone number." appears on the top of the registration form.
 2) No email with OTP code was received.</t>
   </si>
+  <si>
+    <t>Failed Sign in (empty password)</t>
+  </si>
+  <si>
+    <t>Failed Sign in (wrong password)</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>User cant sign in with registered email but wront password</t>
+  </si>
+  <si>
+    <t>User cant sign in with registered email but empty password</t>
+  </si>
+  <si>
+    <t>Validate the behavior and constraints of the "Full Name", "Phone", "Password" and "OTP Verification" fields, during registration.
+Verify correct error messages are showed to the user.
+Min/max field sizes.
+Blank spaces at the start/end of the field.</t>
+  </si>
+  <si>
+    <t>User Verification</t>
+  </si>
+  <si>
+    <t>Random OTP code during registration.</t>
+  </si>
+  <si>
+    <t>OTP code of another registering user during registration</t>
+  </si>
+  <si>
+    <t>During registration, only the actual OTP code that was sent to the user can be used.
+Registration shouldn’t complete with a random OTP code.</t>
+  </si>
+  <si>
+    <t>Interaption during registration (after OTP was sent)</t>
+  </si>
+  <si>
+    <t>Test behavior of closing the browser completly in the middle of the registration process.</t>
+  </si>
+  <si>
+    <t>Sign in with registered account but without OTP verification.</t>
+  </si>
+  <si>
+    <t>After the OTP code was sent, the user opens a new browser and inputs the email + password he registered with.
+Should not be possible (?)</t>
+  </si>
+  <si>
+    <t>Search/Filtering</t>
+  </si>
+  <si>
+    <t>Same search query returns same result</t>
+  </si>
+  <si>
+    <t>When a user uses same keywords/string for 2 searches, the results and their order stays the same.
+Ensures consistancy in site behavior.</t>
+  </si>
+  <si>
+    <t>Search field</t>
+  </si>
+  <si>
+    <t>user experience</t>
+  </si>
+  <si>
+    <t>Multiple Sign in attempts with wrong password</t>
+  </si>
+  <si>
+    <t>If user fails to authenticate multiple times, block account/require password reset</t>
+  </si>
+  <si>
+    <t>The testings to the search field itself is very limited, as we need to know the product requirements to understand the desired behavior.</t>
+  </si>
+  <si>
+    <t>Same results in drop down and search page</t>
+  </si>
+  <si>
+    <t>When user writes the query (and before he confirms it), the drop-down list of suggested products is the same as results after confirming the search.</t>
+  </si>
+  <si>
+    <t>Filters stay when making new search querys</t>
+  </si>
+  <si>
+    <t>User makes a query (like "arduino") and applies it.
+In the results page, he adds filters (like "In Stock", "Top Sale" and "Low to High").
+From the same page, the user sets a new search query (like "rasberry pi").
+New results page is shown for the new queries, the filters from the previous seatch are still on, and the new results are filtered accordingly.</t>
+  </si>
+  <si>
+    <t>Filters</t>
+  </si>
+  <si>
+    <t>This is not the current behavior, but this does make sense.</t>
+  </si>
+  <si>
+    <t>Search results with/without CAPS</t>
+  </si>
+  <si>
+    <t>Same search results for lower cased query and Capitalized query.</t>
+  </si>
+  <si>
+    <t>Individual search filter (Price)</t>
+  </si>
+  <si>
+    <t>Individual search filter (In Stock)</t>
+  </si>
+  <si>
+    <t>Individual search filter (Discount)</t>
+  </si>
+  <si>
+    <t>….</t>
+  </si>
+  <si>
+    <t>Search results with combined filters</t>
+  </si>
+  <si>
+    <t>Brand filters on different search queries</t>
+  </si>
+  <si>
+    <t>Validate that different options are presented under "Brand" filter, for different search queries.</t>
+  </si>
+  <si>
+    <t>apply multiple filters in the search results page and validate the results and their order co-responds to the filters.</t>
+  </si>
+  <si>
+    <t>verify correct result ordering when ordering by "Low to High" and by "High to Low"</t>
+  </si>
+  <si>
+    <t>(can be split into separate tests)</t>
+  </si>
+  <si>
+    <t>Filter reset button</t>
+  </si>
+  <si>
+    <t>After filtering the search results, verify the "Reset button" works as expected</t>
+  </si>
+  <si>
+    <t>Product page</t>
+  </si>
+  <si>
+    <t>moving between product images</t>
+  </si>
+  <si>
+    <t>User can click on different pictures from the picture-gallery and see that picture on screen (+ the smaller picture icon on gallery is highlighted)</t>
+  </si>
+  <si>
+    <t>zooming in/out pictures</t>
+  </si>
+  <si>
+    <t>When user hovers over the picture, a popup with a zoomed in version of the picture is displayed.
+User can use mouse wheel to scroll up (zoom in) or down (zoom out)</t>
+  </si>
+  <si>
+    <t>Basic information on product page</t>
+  </si>
+  <si>
+    <t>Need to verify with product team what information should always be displayed.</t>
+  </si>
+  <si>
+    <t>When users click on a product, a page with the product details and description is showed.
+Verify that the expected details are presented (Picture, title, num of ratings, Qs answered, SKU, Brand, Warranty, Price, Category.</t>
+  </si>
+  <si>
+    <t>Number of answered questions corresponds to the actual visible answered questions</t>
+  </si>
+  <si>
+    <t>The number on the top of the product page ("3 Answered Questions"), is the same as the actual number of visible questions/answers (In the buttom of the page)</t>
+  </si>
+  <si>
+    <t>Number of ratings from the top corresponds to the actual number of reviews</t>
+  </si>
+  <si>
+    <t>Product rating integrity</t>
+  </si>
+  <si>
+    <t>Manually calculate the average rating of the product, and verify it is the same as stated on the top of the page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product page - Navigation buttons </t>
+  </si>
+  <si>
+    <t>Clicking on the "X Ratings" will send the page to ratings section
+Clicking on "X Answered Questions" will send the page to questions section.</t>
+  </si>
+  <si>
+    <t>Adding a question on a product</t>
+  </si>
+  <si>
+    <t>User can add a question on the product page</t>
+  </si>
+  <si>
+    <t>Cart operations</t>
+  </si>
+  <si>
+    <t>Add a product to the cart</t>
+  </si>
+  <si>
+    <t>User can add a product to the cart</t>
+  </si>
+  <si>
+    <t>Add multiple different products to the cart</t>
+  </si>
+  <si>
+    <t>Add multiple quantaties of the same product to cart</t>
+  </si>
+  <si>
+    <t>User can change quantaty on product page and add it to cart.
+He can later view the cart and see the correct number of items</t>
+  </si>
+  <si>
+    <t>User can add multiple quantaties + multiple products to the cart.
+He can later view the cart and see all added products and quantaties</t>
+  </si>
+  <si>
+    <t>Removing an item from the cart</t>
+  </si>
+  <si>
+    <t>User can press the "X" button near an item in his cart to remove all quantities of that item.</t>
+  </si>
+  <si>
+    <t>If user tries to add 999 quantites of a product, it will fix it to the maximum allowed and show an error message.</t>
+  </si>
+  <si>
+    <t>Minimum/Maximum quantities (writing the quantity)</t>
+  </si>
+  <si>
+    <t>Minimum/Maximum quantities (using - +)</t>
+  </si>
+  <si>
+    <t>When user reaches max quantity, pressing on "+" shows error message.
+When user reachse 1, pressing on "-" shows error message.</t>
+  </si>
+  <si>
+    <t>Cart total sum validation</t>
+  </si>
+  <si>
+    <t>When adding multiple items/quantaties, the total "Payable Total" is correct.</t>
+  </si>
+  <si>
+    <t>Empty cart</t>
+  </si>
+  <si>
+    <t>When viewing cart without items, The correct info is present.
+(0 items, total 0, empty product table etc)</t>
+  </si>
+  <si>
+    <t>User Profile</t>
+  </si>
+  <si>
+    <t>Edit Single profile field (First Name)</t>
+  </si>
+  <si>
+    <t>Edit Single profile field (Last Name)</t>
+  </si>
+  <si>
+    <t>Edit Single profile field (City)</t>
+  </si>
+  <si>
+    <t>Edit multiple profile fields</t>
+  </si>
+  <si>
+    <t>User edits multiple different fields in profile and saves.
+Upon closing and opening the page, the data is updated.</t>
+  </si>
+  <si>
+    <t>Editing profile with empty fields</t>
+  </si>
+  <si>
+    <t>User cant leave required fields empty when updating profile.</t>
+  </si>
+  <si>
+    <t>New order is showing in order history</t>
+  </si>
+  <si>
+    <t>User orders a products and verifies it is showing in his "Product Orders" (with "Processing" status)</t>
+  </si>
+  <si>
+    <t>User can change the XXX field and save it.</t>
+  </si>
+  <si>
+    <t>Order details</t>
+  </si>
+  <si>
+    <t>User can click "Details" of a past order and see the details.</t>
+  </si>
+  <si>
+    <t>Order history</t>
+  </si>
+  <si>
+    <t>User profile</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Start registration with EMAIL1 and EMAIL2, and request OTP code for both of them.
+Trying to use the OTP code of EMAIL1 during registration of EMAIL2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>should not be possible.</t>
+    </r>
+  </si>
+  <si>
+    <t>Registration and Authentication</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,19 +650,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Lato"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -377,8 +670,38 @@
       <name val="Lato"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +723,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,7 +861,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -543,9 +872,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -569,124 +895,136 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1045,168 +1383,818 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2607C0-B33A-4A87-8C6B-2CEF4B89D541}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="64" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.42578125" style="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.5703125" style="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+    </row>
+    <row r="3" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="45">
+        <v>1</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="48"/>
+    </row>
+    <row r="4" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="48">
+        <v>2</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="48"/>
+    </row>
+    <row r="5" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="48">
+        <v>3</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="48"/>
+    </row>
+    <row r="6" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="45">
+        <v>4</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="48"/>
+    </row>
+    <row r="7" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="48">
+        <v>5</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="48"/>
+      <c r="F7" s="49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="48">
+        <v>6</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="48"/>
+    </row>
+    <row r="9" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="45">
+        <v>7</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="48"/>
+    </row>
+    <row r="10" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="48">
+        <v>8</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="48"/>
+    </row>
+    <row r="11" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="48">
+        <v>9</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="45">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B12" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="48">
+        <v>11</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+    </row>
+    <row r="15" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="48">
+        <v>12</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="48">
+        <v>13</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="48">
+        <v>14</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="48">
         <v>15</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B18" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+    </row>
+    <row r="21" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="48">
+        <v>16</v>
+      </c>
+      <c r="B21" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="48"/>
+    </row>
+    <row r="22" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="48">
+        <v>17</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="48">
+        <v>18</v>
+      </c>
+      <c r="B23" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="111" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="48">
+        <v>19</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="48">
+        <v>20</v>
+      </c>
+      <c r="B25" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="48">
+        <v>21</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="48">
+        <v>22</v>
+      </c>
+      <c r="B27" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="48">
+        <v>23</v>
+      </c>
+      <c r="B28" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="48">
+        <v>24</v>
+      </c>
+      <c r="B29" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="48">
+        <v>25</v>
+      </c>
+      <c r="B30" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="48">
+        <v>26</v>
+      </c>
+      <c r="B31" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="53"/>
+    </row>
+    <row r="33" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="48">
+        <v>27</v>
+      </c>
+      <c r="B33" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="48">
+        <v>28</v>
+      </c>
+      <c r="B34" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="48">
+        <v>29</v>
+      </c>
+      <c r="B35" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="48">
+        <v>30</v>
+      </c>
+      <c r="B36" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="48">
+        <v>31</v>
+      </c>
+      <c r="B37" s="48" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="48">
+        <v>32</v>
+      </c>
+      <c r="B38" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="48">
+        <v>33</v>
+      </c>
+      <c r="B39" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="48">
+        <v>34</v>
+      </c>
+      <c r="B40" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" s="55"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="53"/>
+    </row>
+    <row r="42" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="48">
         <v>35</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="24" t="s">
+      <c r="B42" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="47" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="48">
+        <v>36</v>
+      </c>
+      <c r="B43" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="47" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="48">
+        <v>37</v>
+      </c>
+      <c r="B44" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="48">
+        <v>38</v>
+      </c>
+      <c r="B45" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" s="47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="48">
+        <v>39</v>
+      </c>
+      <c r="B46" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C46" s="47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="48">
+        <v>40</v>
+      </c>
+      <c r="B47" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="48">
+        <v>41</v>
+      </c>
+      <c r="B48" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" s="47" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="48">
+        <v>42</v>
+      </c>
+      <c r="B49" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" s="47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="B50" s="55"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="53"/>
+    </row>
+    <row r="51" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="48">
+        <v>43</v>
+      </c>
+      <c r="B51" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D51" s="48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="48">
+        <v>44</v>
+      </c>
+      <c r="B52" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="C52" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" s="48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="48">
         <v>45</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="B53" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="48">
         <v>46</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="B55" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="C55" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" s="48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="48">
         <v>47</v>
       </c>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="6" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17">
-        <v>4</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="14"/>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17">
-        <v>5</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="14"/>
-    </row>
-    <row r="9" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
-        <v>6</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="14"/>
-    </row>
-    <row r="10" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17">
-        <v>7</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
-        <v>8</v>
-      </c>
-    </row>
+      <c r="B56" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="D56" s="48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="48">
+        <v>48</v>
+      </c>
+      <c r="B57" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="D57" s="48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="48">
+        <v>48</v>
+      </c>
+      <c r="B58" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="C58" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" s="48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="B59" s="54"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="54"/>
+      <c r="F59" s="54"/>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="66" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A59:F59"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A41:F41"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1215,48 +2203,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FBFEDB-FA26-47D2-8CE6-2036C94BD4AC}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="6.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="88.140625" style="23" customWidth="1"/>
-    <col min="8" max="8" width="111.7109375" style="23" customWidth="1"/>
+    <col min="7" max="7" width="88.140625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="111.7109375" style="13" customWidth="1"/>
     <col min="9" max="13" width="15.7109375" style="3" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="47" t="s">
+      <c r="A1" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="25" t="s">
-        <v>58</v>
+      <c r="F1" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>5</v>
@@ -1275,250 +2263,246 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26">
+      <c r="A2" s="36">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28">
+      <c r="B2" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="15">
         <v>1</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="36"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="15">
+        <v>2</v>
+      </c>
+      <c r="G3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28">
-        <v>2</v>
-      </c>
-      <c r="G3" s="30" t="s">
+      <c r="H3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="42"/>
+    </row>
+    <row r="4" spans="1:13" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="36"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="15">
+        <v>3</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="33"/>
-    </row>
-    <row r="4" spans="1:13" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28">
-        <v>3</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="42"/>
+    </row>
+    <row r="5" spans="1:13" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="36"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="15">
+        <v>4</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="33"/>
-    </row>
-    <row r="5" spans="1:13" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28">
-        <v>4</v>
-      </c>
-      <c r="G5" s="36" t="s">
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="42"/>
+    </row>
+    <row r="6" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="36"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="15">
+        <v>5</v>
+      </c>
+      <c r="G6" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H6" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="42"/>
+    </row>
+    <row r="7" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="15">
+        <v>6</v>
+      </c>
+      <c r="G7" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="33"/>
-    </row>
-    <row r="6" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28">
-        <v>5</v>
-      </c>
-      <c r="G6" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="37" t="s">
+      <c r="H7" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="33"/>
-    </row>
-    <row r="7" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28">
-        <v>6</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="33"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="42"/>
     </row>
     <row r="8" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="39"/>
-      <c r="C8" s="46"/>
+      <c r="C8" s="41"/>
       <c r="D8" s="39"/>
       <c r="E8" s="39"/>
-      <c r="F8" s="40">
+      <c r="F8" s="24">
         <v>7</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="43"/>
+    </row>
+    <row r="9" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="29">
+        <v>6</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="32">
+        <v>1</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="32">
+        <v>2</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+    </row>
+    <row r="11" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="32">
+        <v>3</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H14" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="H8" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="44"/>
-    </row>
-    <row r="9" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="48">
-        <v>6</v>
-      </c>
-      <c r="B9" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="48"/>
-      <c r="F9" s="51">
-        <v>1</v>
-      </c>
-      <c r="G9" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="51">
-        <v>2</v>
-      </c>
-      <c r="G10" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-    </row>
-    <row r="11" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="51">
-        <v>3</v>
-      </c>
-      <c r="G11" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="54" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H14" s="23" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="M2:M8"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="C2:C8"/>
     <mergeCell ref="D2:D8"/>
     <mergeCell ref="E2:E8"/>
-    <mergeCell ref="M2:M8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="Go to the web site https://techshopbd.com/" xr:uid="{D0D98396-E89F-4498-BC22-79FF13FA3777}"/>
@@ -1545,95 +2529,95 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="13"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>